<commit_message>
Routine BiuBiuGame development, Player control.
</commit_message>
<xml_diff>
--- a/Excel2FlatBuffers/ExcelTable/GamePlay.xlsx
+++ b/Excel2FlatBuffers/ExcelTable/GamePlay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\UnityProject\BiuBiu\Excel2FlatBuffers\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBF43EE-447C-4BDC-AC12-4AF558E972B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFCB2F7-D406-4D99-8289-463F2A219B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28095" yWindow="6405" windowWidth="27435" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>skip</t>
   </si>
@@ -147,6 +147,18 @@
   </si>
   <si>
     <t>PreloadAssets</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>主角资源</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerAsset</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -584,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -597,17 +609,18 @@
     <col min="3" max="3" width="22.625" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
     <col min="5" max="5" width="58" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
-    <col min="9" max="9" width="38.25" customWidth="1"/>
+    <col min="6" max="6" width="32.375" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="9" width="19.5" customWidth="1"/>
+    <col min="10" max="10" width="38.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -623,11 +636,14 @@
       <c r="E2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -643,9 +659,12 @@
       <c r="E3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="F3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
         <v>4</v>
@@ -659,8 +678,11 @@
       <c r="E4" s="13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="127.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F4" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="6">
         <v>1</v>
       </c>
@@ -672,53 +694,56 @@
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F20" s="9"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G20" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>